<commit_message>
#85 #88 updates to fix tests
</commit_message>
<xml_diff>
--- a/inst/extdata/adams-specs.xlsx
+++ b/inst/extdata/adams-specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mancinie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18B75A6-0B75-4EBC-939B-ABA8D3F3FDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4753264-6677-4BCA-909C-29987DE18E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16193" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16193" uniqueCount="1308">
   <si>
     <t>Attribute</t>
   </si>
@@ -3954,9 +3954,6 @@
   </si>
   <si>
     <t>Temporary Height at Timepoint Units</t>
-  </si>
-  <si>
-    <t>Evalutator</t>
   </si>
   <si>
     <t>Vital Signs Analysis for Pediatrics</t>
@@ -5977,7 +5974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -6713,7 +6710,7 @@
         <v>1295</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C24" s="23" t="s">
         <v>35</v>
@@ -6754,8 +6751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1879"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I1800" sqref="I1800:V1801"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1790" workbookViewId="0">
+      <selection activeCell="E1800" sqref="E1800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -78811,7 +78808,7 @@
         <v>1296</v>
       </c>
       <c r="D1804" s="8" t="s">
-        <v>1307</v>
+        <v>745</v>
       </c>
       <c r="E1804" s="8" t="s">
         <v>92</v>

</xml_diff>